<commit_message>
add quick copy template
</commit_message>
<xml_diff>
--- a/doc41/task-status-tracking-template.xlsx
+++ b/doc41/task-status-tracking-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\okay-examples\doc41\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B311862B-B224-4D3A-BEEB-9B50B0866CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72666F6C-D460-4AF0-9001-2FE2772D9D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,40 +26,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t xml:space="preserve">  ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t xml:space="preserve">  Category</t>
   </si>
   <si>
-    <t xml:space="preserve">  Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ETA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Remark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Jira ID</t>
-  </si>
-  <si>
     <t>This user research requires the completion of 20 valid questionnaires within 3 days (SMART), with the aim of providing a basis for product optimization in the next quarter (Context). Please synchronize 5 samples questionnaires to me for direction confirmation by noon on Wednesday (Checkpoint). If there are difficulties in recruiting respondents, you can apply for a budget to increase the incentive of gifts(Contingency).</t>
   </si>
   <si>
-    <t>Priority 
-(High:1/Medium:2/Low:3)</t>
-  </si>
-  <si>
-    <t>Due to (Why), (Who) need to do (How much) of (What) at (Where) in (Scope) by (When), otherwise (Consequence), here is (How) and (Resources) for reference.</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ETA</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Priority(High:1/Medium:2/Low:3)</t>
+  </si>
+  <si>
+    <t>JiraID</t>
+  </si>
+  <si>
+    <t>Due to (Why), (Who) requires (How much) of (What) at (Where) in (Scope) by (When), otherwise (Consequence), here is (How) and (Resources) for reference.</t>
   </si>
 </sst>
 </file>
@@ -420,7 +419,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -440,31 +439,31 @@
   <sheetData>
     <row r="1" spans="1:13" ht="41" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="J1" s="3">
         <v>45774</v>
@@ -484,7 +483,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -820,12 +819,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5372E79A-0A92-410C-A3A4-38E2375806D2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="29.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="28">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>